<commit_message>
added links for range in graph
</commit_message>
<xml_diff>
--- a/tests/ast/pruning.xlsx
+++ b/tests/ast/pruning.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="test">Sheet1!$G$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -382,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -390,7 +393,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1">
         <v>1</v>
       </c>
@@ -403,8 +406,17 @@
       <c r="D1">
         <v>9</v>
       </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
@@ -418,16 +430,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:9">
       <c r="A3">
         <f>A2+B2</f>
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:9">
       <c r="C6">
-        <f>A3+D2</f>
-        <v>23</v>
+        <f>A3+D2+H1</f>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>